<commit_message>
Create autodraft option and add byes and ESPN projections to draft histories and depth charts
</commit_message>
<xml_diff>
--- a/depth_chart_blank.xlsx
+++ b/depth_chart_blank.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew\Documents\Fantasy Football\SJP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benderas/Documents/Fantasy Football/sjp_ff/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4C61E92F-4690-42CE-A332-631E615D3DB5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D207F28-FF0F-C64E-9E80-B5AE22C2EBEB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="11530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="21600" windowHeight="11540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>QB</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t>Bench7</t>
+  </si>
+  <si>
+    <t>Bye</t>
+  </si>
+  <si>
+    <t>ESPN Projection</t>
   </si>
 </sst>
 </file>
@@ -430,98 +436,104 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Begin implementing salary cap format
</commit_message>
<xml_diff>
--- a/depth_chart_blank.xlsx
+++ b/depth_chart_blank.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benderas/Documents/Fantasy Football/sjp_ff/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D207F28-FF0F-C64E-9E80-B5AE22C2EBEB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80910FF6-829E-A449-BA5D-49D8CC9676F5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="21600" windowHeight="11540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-35300" yWindow="4420" windowWidth="21600" windowHeight="11540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>QB</t>
   </si>
@@ -85,19 +85,33 @@
   </si>
   <si>
     <t>ESPN Projection</t>
+  </si>
+  <si>
+    <t>Salary</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>Team</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -120,8 +134,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,99 +452,108 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>16</v>
       </c>

</xml_diff>